<commit_message>
[Dev] Supplier & SupplierRevision - 增加調整欄位title說明
</commit_message>
<xml_diff>
--- a/Platform/Platform.WebSite/ModuleResources/Other/Supplier/新增供應商匯入範本.xlsx
+++ b/Platform/Platform.WebSite/ModuleResources/Other/Supplier/新增供應商匯入範本.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\加鑫科技\1.1 客戶報價單\新竹_TET\供應商平台&amp;評鑑\系統開發\Dev\Platform\Platform.WebSite\ModuleResources\Other\Supplier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nkp07\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{662B206E-1630-4769-8840-5BB6B0E30BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189D0DE0-43F5-4E5F-9A35-CD19B8E85A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12504" xr2:uid="{9CCFBBE6-BC22-49C3-84C8-F09A8799A7EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9CCFBBE6-BC22-49C3-84C8-F09A8799A7EF}"/>
   </bookViews>
   <sheets>
     <sheet name="供應商資料" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>SWIFT CODE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1580,9 +1580,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>請填寫英文地址</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1665,6 +1662,26 @@
       </rPr>
       <t>USD</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外幣帳戶請填英文帳戶名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請填寫英文地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請填寫城市英文名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外幣帳戶必填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>若為外幣匯款，請以英文填寫公司地址</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2002,7 +2019,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -2678,19 +2695,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14990691854609822"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
       </left>
@@ -2735,7 +2739,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2844,13 +2848,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="3" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="3" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2880,6 +2884,84 @@
     <xf numFmtId="49" fontId="39" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="26" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="4" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="20" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2889,15 +2971,6 @@
     <xf numFmtId="49" fontId="20" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="19" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2907,83 +2980,11 @@
     <xf numFmtId="49" fontId="19" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="3" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3122,8 +3123,8 @@
       <xdr:rowOff>98424</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>324485</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1315085</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>612479</xdr:rowOff>
     </xdr:to>
@@ -3460,14 +3461,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC91742-CCA7-4F0A-A44A-A37494EA795C}">
   <dimension ref="A2:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="3.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="37.21875" style="1" customWidth="1"/>
     <col min="5" max="6" width="16.88671875" style="1" customWidth="1"/>
@@ -3476,31 +3477,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="52.5" customHeight="1">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="1:7" ht="120" customHeight="1" thickBot="1">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="79"/>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="38.549999999999997" customHeight="1" thickTop="1">
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="38.700000000000003" customHeight="1" thickTop="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="71"/>
+      <c r="C4" s="66"/>
       <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
@@ -3509,12 +3510,12 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="38.549999999999997" customHeight="1">
+    <row r="5" spans="1:7" ht="38.700000000000003" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="64"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
         <v>22</v>
@@ -3524,7 +3525,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="38.549999999999997" customHeight="1">
+    <row r="6" spans="1:7" ht="38.700000000000003" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="12" t="s">
         <v>5</v>
@@ -3539,12 +3540,12 @@
       <c r="F6" s="16"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="38.549999999999997" customHeight="1">
+    <row r="7" spans="1:7" ht="38.700000000000003" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="64"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="14"/>
       <c r="E7" s="17" t="s">
         <v>24</v>
@@ -3552,12 +3553,12 @@
       <c r="F7" s="18"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="38.549999999999997" customHeight="1">
+    <row r="8" spans="1:7" ht="38.700000000000003" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="64"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="14"/>
       <c r="E8" s="17" t="s">
         <v>25</v>
@@ -3565,70 +3566,72 @@
       <c r="F8" s="18"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="38.549999999999997" customHeight="1">
+    <row r="9" spans="1:7" ht="38.700000000000003" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="64"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="19"/>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="66"/>
+      <c r="F9" s="61"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="38.549999999999997" customHeight="1">
+    <row r="10" spans="1:7" ht="38.700000000000003" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="64"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="20"/>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="64"/>
+      <c r="F10" s="59"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" ht="38.549999999999997" customHeight="1">
+    <row r="11" spans="1:7" ht="38.700000000000003" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="73"/>
+      <c r="C11" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="D11" s="21"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="69"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="64"/>
     </row>
     <row r="12" spans="1:7" ht="25.95" customHeight="1" thickBot="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="81"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="73"/>
     </row>
-    <row r="13" spans="1:7" ht="38.549999999999997" customHeight="1" thickTop="1" thickBot="1">
+    <row r="13" spans="1:7" ht="38.700000000000003" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="57"/>
     </row>
     <row r="14" spans="1:7" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="75"/>
+      <c r="C14" s="68"/>
       <c r="D14" s="22"/>
       <c r="E14" s="40" t="s">
         <v>13</v>
@@ -3639,10 +3642,10 @@
       <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" ht="31.5" customHeight="1" thickTop="1">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="77"/>
+      <c r="C15" s="70"/>
       <c r="D15" s="24"/>
       <c r="E15" s="25" t="s">
         <v>15</v>
@@ -3653,20 +3656,22 @@
       <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" ht="31.5" customHeight="1">
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="78"/>
+      <c r="C16" s="41" t="s">
+        <v>45</v>
+      </c>
       <c r="D16" s="26"/>
       <c r="E16" s="25" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="2:7" ht="37.799999999999997" customHeight="1" thickBot="1">
+    <row r="17" spans="2:7" ht="37.950000000000003" customHeight="1" thickBot="1">
       <c r="B17" s="39" t="s">
         <v>32</v>
       </c>
@@ -3678,30 +3683,34 @@
         <v>31</v>
       </c>
       <c r="F17" s="47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="29"/>
     </row>
     <row r="18" spans="2:7" ht="28.95" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="50"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="76"/>
     </row>
     <row r="19" spans="2:7" ht="31.5" customHeight="1" thickTop="1">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="53"/>
+      <c r="C19" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="D19" s="27"/>
-      <c r="E19" s="51" t="s">
+      <c r="E19" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="51"/>
+      <c r="F19" s="41" t="s">
+        <v>48</v>
+      </c>
       <c r="G19" s="30"/>
     </row>
     <row r="20" spans="2:7" ht="31.5" customHeight="1" thickBot="1">
@@ -3709,7 +3718,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D20" s="31"/>
       <c r="E20" s="32"/>
@@ -3726,14 +3735,11 @@
     <protectedRange algorithmName="SHA-512" hashValue="BvMNEMOrSVRp6QLR5OEsD6Pgwtai1ERy7EKAeN1vw7pzwLng5A5fRHPTEXazPIDkvmC544x2F1EMtTB2PIcnWQ==" saltValue="J0w7XMK8Kt5HxE600AFkpw==" spinCount="100000" sqref="G16" name="範圍1_4"/>
     <protectedRange algorithmName="SHA-512" hashValue="BvMNEMOrSVRp6QLR5OEsD6Pgwtai1ERy7EKAeN1vw7pzwLng5A5fRHPTEXazPIDkvmC544x2F1EMtTB2PIcnWQ==" saltValue="J0w7XMK8Kt5HxE600AFkpw==" spinCount="100000" sqref="G17" name="範圍1_5"/>
   </protectedRanges>
-  <mergeCells count="20">
+  <mergeCells count="16">
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B13:G13"/>
@@ -3746,7 +3752,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
@@ -3777,7 +3782,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="16.44140625" style="35" customWidth="1"/>
     <col min="2" max="2" width="22" style="35" customWidth="1"/>
@@ -3788,13 +3793,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:5" ht="27.6" thickTop="1">
       <c r="A2" s="36" t="s">

</xml_diff>